<commit_message>
Update on the dashboard
</commit_message>
<xml_diff>
--- a/Project Management Dashboard.xlsx
+++ b/Project Management Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walid\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34E9152-2982-46F7-B896-C0B8654C061E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A7CCB4-EAFE-47F5-8461-98D5135FC28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="664" xr2:uid="{599CBDBA-6DCB-491A-8F55-440439BE8440}"/>
   </bookViews>
@@ -16,8 +16,7 @@
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
     <sheet name="Workings" sheetId="4" r:id="rId2"/>
     <sheet name="Instructions" sheetId="6" r:id="rId3"/>
-    <sheet name="Dashboard Protection" sheetId="9" r:id="rId4"/>
-    <sheet name="Data" sheetId="1" r:id="rId5"/>
+    <sheet name="Data" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Dashboard!$A$1:$X$46</definedName>
@@ -26,13 +25,13 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
       <x14:slicerCaches>
+        <x14:slicerCache r:id="rId6"/>
         <x14:slicerCache r:id="rId7"/>
-        <x14:slicerCache r:id="rId8"/>
       </x14:slicerCaches>
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="97">
   <si>
     <t>Project</t>
   </si>
@@ -329,9 +328,6 @@
     <t>Bar chart height 3.73 x 9.0 wide.</t>
   </si>
   <si>
-    <t>Protecting your dashboard</t>
-  </si>
-  <si>
     <t>Gantt Chart - Conditional Formatting (extend the 'applies to' range to allow for growth in your data)</t>
   </si>
   <si>
@@ -366,13 +362,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0\ &quot;Days&quot;"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="#,##0.0,,&quot;M&quot;"/>
-    <numFmt numFmtId="168" formatCode="\▼0.0%;\▼0.0%"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,28 +449,8 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
-      <color theme="0"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -491,12 +466,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF336600"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,7 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -646,18 +615,456 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="64">
+  <dxfs count="164">
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
@@ -686,10 +1093,10 @@
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="d/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode="d/mm/yyyy"/>
+      <numFmt numFmtId="168" formatCode="d/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="d/mm/yyyy"/>
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
@@ -1018,8 +1425,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="No Border" pivot="0" table="0" count="10" xr9:uid="{EEEA172B-89F3-489D-B80E-D598FE9BFA19}">
-      <tableStyleElement type="wholeTable" dxfId="63"/>
-      <tableStyleElement type="headerRow" dxfId="62"/>
+      <tableStyleElement type="wholeTable" dxfId="163"/>
+      <tableStyleElement type="headerRow" dxfId="162"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1477,7 +1884,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[project_management_dashboard_non_365.xlsx]Workings!Budget_v_Actual</c:name>
+    <c:name>[Project Management Dashboard.xlsx]Workings!Budget_v_Actual</c:name>
     <c:fmtId val="21"/>
   </c:pivotSource>
   <c:chart>
@@ -5432,7 +5839,7 @@
             <xdr:cNvPr id="8" name="Manager">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5510,7 +5917,7 @@
             <xdr:cNvPr id="3" name="Project">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5586,7 +5993,7 @@
         <xdr:cNvPr id="14" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5624,7 +6031,7 @@
         <xdr:cNvPr id="18" name="Chart 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5667,7 +6074,7 @@
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5712,7 +6119,7 @@
         <xdr:cNvPr id="19" name="Chart 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5750,7 +6157,7 @@
         <xdr:cNvPr id="20" name="Chart 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5788,7 +6195,7 @@
         <xdr:cNvPr id="11" name="TextBox 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6172,7 +6579,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6223,7 +6630,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6274,7 +6681,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6342,7 +6749,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6393,7 +6800,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6444,7 +6851,7 @@
         <xdr:cNvPr id="11" name="Picture 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6495,7 +6902,7 @@
         <xdr:cNvPr id="12" name="Picture 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6546,7 +6953,7 @@
         <xdr:cNvPr id="13" name="Picture 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6597,7 +7004,7 @@
         <xdr:cNvPr id="14" name="Picture 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6648,7 +7055,7 @@
         <xdr:cNvPr id="15" name="Picture 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6699,7 +7106,7 @@
         <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000010000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000010000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6750,7 +7157,7 @@
         <xdr:cNvPr id="18" name="Picture 17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000012000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6801,7 +7208,7 @@
         <xdr:cNvPr id="19" name="Picture 18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000013000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000013000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6852,7 +7259,7 @@
         <xdr:cNvPr id="20" name="Picture 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000014000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000014000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6903,7 +7310,7 @@
         <xdr:cNvPr id="21" name="Picture 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6954,7 +7361,7 @@
         <xdr:cNvPr id="22" name="Picture 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7005,7 +7412,7 @@
         <xdr:cNvPr id="25" name="Picture 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7056,7 +7463,7 @@
         <xdr:cNvPr id="28" name="Picture 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7107,7 +7514,7 @@
         <xdr:cNvPr id="30" name="Picture 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7158,7 +7565,7 @@
         <xdr:cNvPr id="31" name="Picture 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7202,7 +7609,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7253,7 +7660,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7304,7 +7711,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7355,7 +7762,7 @@
         <xdr:cNvPr id="10" name="Picture 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7406,7 +7813,7 @@
         <xdr:cNvPr id="17" name="Picture 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000011000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000011000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7457,7 +7864,7 @@
         <xdr:cNvPr id="23" name="Picture 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7508,7 +7915,7 @@
         <xdr:cNvPr id="24" name="Picture 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7544,1351 +7951,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
+      <xdr:colOff>581025</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="32" name="Group 31">
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Graphic 26" descr="Video camera">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000020000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="5362575" y="304800"/>
-          <a:ext cx="3333750" cy="914400"/>
-          <a:chOff x="5362575" y="304800"/>
-          <a:chExt cx="3333750" cy="914400"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="29" name="Rectangle: Rounded Corners 28">
-            <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28"/>
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001D000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5362575" y="333375"/>
-            <a:ext cx="3333750" cy="857250"/>
-          </a:xfrm>
-          <a:prstGeom prst="roundRect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent2">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="accent2"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent2"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="lt1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="r"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="2000"/>
-              <a:t>CLICK</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="2000" baseline="0"/>
-              <a:t> TO </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="2000"/>
-              <a:t>WATCH THE</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:pPr algn="r"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="2000"/>
-              <a:t>VIDEO TUTORIAL</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="27" name="Graphic 26" descr="Video camera">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001B000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-              <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-                <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId30"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5457825" y="304800"/>
-            <a:ext cx="914400" cy="914400"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-      </xdr:pic>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="276225" y="4638675"/>
-          <a:ext cx="5943600" cy="3286124"/>
-          <a:chOff x="276225" y="4286250"/>
-          <a:chExt cx="6629400" cy="3714749"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="TextBox 2">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="276225" y="4286250"/>
-            <a:ext cx="6629400" cy="3714749"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1800">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>2. Worksheet Protection - </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>You'll find the Worksheet Protection on the Review tab:</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-AU" sz="1800">
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="r"/>
-            <a:endParaRPr lang="en-AU" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="r"/>
-            <a:endParaRPr lang="en-AU" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="r"/>
-            <a:endParaRPr lang="en-AU" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:pPr algn="r"/>
-            <a:endParaRPr lang="en-AU" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="4" name="Picture 3" descr="C:\Users\Mynda\AppData\Local\Temp\SNAGHTML16e4b49.PNG">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="542925" y="5079326"/>
-            <a:ext cx="2600325" cy="2835077"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:effectLst>
-            <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="40000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="5" name="Group 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="276225" y="752474"/>
-          <a:ext cx="11220450" cy="3771901"/>
-          <a:chOff x="276225" y="676274"/>
-          <a:chExt cx="12515850" cy="4067176"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="TextBox 5">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="276225" y="676274"/>
-            <a:ext cx="6629400" cy="4067176"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1800">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>1. Slicers - </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>prevent users activating the pull handles when using the Slicer by selecting 'Disable resizing and moving' in the Slicer Position and Layout setting (right-click Slicer).</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="7" name="Picture 6">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000007000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2209800" y="2319360"/>
-            <a:ext cx="2552381" cy="2123810"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:effectLst>
-            <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="40000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="8" name="Picture 7" descr="C:\Users\Mynda\AppData\Local\Temp\SNAGHTML1864985.PNG">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000008000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="523875" y="1729269"/>
-            <a:ext cx="1419048" cy="2780952"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="9" name="TextBox 8">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000009000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7000875" y="676274"/>
-            <a:ext cx="5791200" cy="4067176"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1800">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Or</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1800" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1800">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Slicers - </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Simply</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t> protect the worksheet containing the Dashboard, but make sure you 'unprotect' Slicers so that they can still be clicked:</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-AU" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="10" name="Picture 9" descr="C:\Users\Mynda\AppData\Local\Temp\SNAGHTML1a10d60.PNG">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000A000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="5286375" y="1695450"/>
-            <a:ext cx="1466667" cy="2828571"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="11" name="TextBox 10">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000B000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="352425" y="1381125"/>
-            <a:ext cx="1695450" cy="314325"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1100"/>
-              <a:t>Before Disabling Resizing</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="12" name="TextBox 11">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000C000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="5057775" y="1381125"/>
-            <a:ext cx="1695450" cy="314325"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr"/>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1100"/>
-              <a:t>After Disabling Resizing</a:t>
-            </a:r>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="13" name="Picture 12">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000D000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="8543925" y="1400175"/>
-            <a:ext cx="2542857" cy="3057143"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:effectLst>
-            <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="40000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </xdr:spPr>
-      </xdr:pic>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="TextBox 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000E000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3124200" y="6219825"/>
-          <a:ext cx="2933700" cy="1514475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>If your Dashboard sheet</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> contains a PivotTable,</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> make sure 'Use PivotTable &amp; PivotChart' is  checked so that Slicers work.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-AU">
-            <a:effectLst/>
-            <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>Note</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>, this will prevent the PivotTables in the entire file from being refreshed,</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-AU" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t> so if you're planning on updating your dashboard with new data, then option 3 is preferred.</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-AU">
-            <a:effectLst/>
-            <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>90140</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="15" name="Group 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-00000F000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="276225" y="11196290"/>
-          <a:ext cx="5943600" cy="3510311"/>
-          <a:chOff x="276225" y="12358340"/>
-          <a:chExt cx="6629400" cy="3596036"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="16" name="TextBox 15">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000010000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="276225" y="12358340"/>
-            <a:ext cx="6629400" cy="3596036"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1800">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>4. Protect</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1800" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t> Workbook</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-AU" sz="1800">
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Once</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t> you've 'VeryHidden' the sheets containing your workings and data you need to protect your workbook so your users can't unhide them.</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-AU" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-AU" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-AU" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-AU" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-AU" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-AU" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-AU" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="FF0000"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>WARNING</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>: this protection is not bullet proof. If a user wants to get to your underlying data they can find a way. A Google search will reveal various ways to crack your password, or simply remove the protection. </a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-AU" sz="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Therefore Worksheet Protection should be used to prevent users breaking your report, but don't count on it protecting super sensitive information.</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-AU" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="17" name="Picture 16" descr="C:\Users\Mynda\AppData\Local\Temp\SNAGHTML1be30b9.PNG">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000011000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="2162175" y="13351281"/>
-            <a:ext cx="2238375" cy="1000125"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:effectLst>
-            <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="40000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1980924" cy="1000000"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000012000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8897,362 +7975,13 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3505200" y="5086350"/>
-          <a:ext cx="1980924" cy="1000000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>184231</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="19" name="Group 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000013000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="276225" y="8086725"/>
-          <a:ext cx="5943600" cy="3013156"/>
-          <a:chOff x="276225" y="8820150"/>
-          <a:chExt cx="6629400" cy="3441781"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="20" name="TextBox 19">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000014000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="276225" y="8820150"/>
-            <a:ext cx="6629400" cy="3441781"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:solidFill>
-            <a:schemeClr val="lt1"/>
-          </a:solidFill>
-          <a:ln w="9525" cmpd="sng">
-            <a:solidFill>
-              <a:schemeClr val="lt1">
-                <a:shade val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1800">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="50000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>3. Hide Worksheets</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>A better solution is to set the property for the </a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>sheets containing your data and workings to </a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>VeryHidden in the VB Editor Alt+F11.</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:endParaRPr lang="en-AU" sz="800">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>When you right-click</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t> the sheet tab there is no</a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>indication that worksheets are hidden when </a:t>
-            </a:r>
-          </a:p>
-          <a:p>
-            <a:r>
-              <a:rPr lang="en-AU" sz="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>their properties are set to 'xlSheetVeryHidden'</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-AU" sz="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Segoe UI" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="21" name="Picture 20" descr="C:\Users\Mynda\AppData\Local\Temp\SNAGHTML1822ee4.PNG">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000015000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="3810000" y="8985432"/>
-            <a:ext cx="2847975" cy="3140383"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:effectLst>
-            <a:outerShdw blurRad="63500" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="40000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="22" name="Picture 21" descr="C:\Users\Mynda\AppData\Local\Temp\SNAGHTML1c4ed53.PNG">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000016000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
-            <a:extLst>
-              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-              </a:ext>
-            </a:extLst>
-          </a:blip>
-          <a:srcRect/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="800100" y="10534650"/>
-            <a:ext cx="2066925" cy="1676400"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:effectLst>
-            <a:outerShdw blurRad="50800" dist="38100" dir="16200000" rotWithShape="0">
-              <a:prstClr val="black">
-                <a:alpha val="40000"/>
-              </a:prstClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:extLst>
-            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-                <a:solidFill>
-                  <a:srgbClr val="FFFFFF"/>
-                </a:solidFill>
-              </a14:hiddenFill>
-            </a:ext>
-          </a:extLst>
-        </xdr:spPr>
-      </xdr:pic>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3230281" cy="533616"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Picture 23">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000018000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId29"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -9262,8 +7991,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9620250" y="47625"/>
-          <a:ext cx="3230281" cy="533616"/>
+          <a:off x="5457825" y="304800"/>
+          <a:ext cx="914400" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9271,7 +8000,7 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9895,7 +8624,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B155B9DB-4CE8-497A-978F-D31E4BA07222}" name="Gantt" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B155B9DB-4CE8-497A-978F-D31E4BA07222}" name="Gantt" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A5:J46" firstHeaderRow="0" firstDataRow="1" firstDataCol="8"/>
   <pivotFields count="10">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
@@ -10410,7 +9139,7 @@
     <dataField name="Actual " fld="9" baseField="0" baseItem="2" numFmtId="3"/>
   </dataFields>
   <formats count="50">
-    <format dxfId="55">
+    <format dxfId="155">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -10420,46 +9149,46 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="154">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="153">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="152">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="151">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="150">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="149">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="148">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="147">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="146">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="45">
+    <format dxfId="145">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="144">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="143">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="42">
+    <format dxfId="142">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="141">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -10469,31 +9198,31 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="140">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="139">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="138">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="137">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="136">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="135">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="134">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="133">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="132">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -10503,31 +9232,31 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="131">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="130">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="129">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="28">
+    <format dxfId="128">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="27">
+    <format dxfId="127">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="26">
+    <format dxfId="126">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="25">
+    <format dxfId="125">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="24">
+    <format dxfId="124">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="23">
+    <format dxfId="123">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -10537,31 +9266,31 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="122">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="121">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="120">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
     </format>
-    <format dxfId="19">
+    <format dxfId="119">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="3"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="118">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="117">
       <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="4"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="116">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="115">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="114">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -10571,19 +9300,19 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="13">
+    <format dxfId="113">
       <pivotArea field="4" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="5"/>
     </format>
-    <format dxfId="12">
+    <format dxfId="112">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="6"/>
     </format>
-    <format dxfId="11">
+    <format dxfId="111">
       <pivotArea field="7" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="7"/>
     </format>
-    <format dxfId="10">
+    <format dxfId="110">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="9">
+    <format dxfId="109">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="8">
           <reference field="0" count="1" selected="0">
@@ -10613,7 +9342,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="8">
+    <format dxfId="108">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="8">
           <reference field="0" count="1" selected="0">
@@ -10643,14 +9372,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="7">
+    <format dxfId="107">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="6" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="6">
+    <format dxfId="106">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4" count="0"/>
@@ -10671,70 +9400,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EABCFFF3-195F-4C92-8A2E-C048CA24D4C9}" name="Days_Completed" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
-  <location ref="I2:J4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="4"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="4"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField dataField="1" numFmtId="3" showAll="0"/>
-    <pivotField numFmtId="9" showAll="0"/>
-    <pivotField numFmtId="3" showAll="0"/>
-    <pivotField numFmtId="3" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="2">
-    <dataField name="Days completed " fld="6" baseField="0" baseItem="0"/>
-    <dataField name="Duration " fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DDFB2C1-F4B8-49AF-A1F4-4361E5203E0E}" name="Budget_v_Actual" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8DDFB2C1-F4B8-49AF-A1F4-4361E5203E0E}" name="Budget_v_Actual" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="24">
   <location ref="B2:C3" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="10">
     <pivotField showAll="0">
@@ -10861,6 +9527,69 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EABCFFF3-195F-4C92-8A2E-C048CA24D4C9}" name="Days_Completed" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="6">
+  <location ref="I2:J4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" numFmtId="3" showAll="0"/>
+    <pivotField numFmtId="9" showAll="0"/>
+    <pivotField numFmtId="3" showAll="0"/>
+    <pivotField numFmtId="3" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Days completed " fld="6" baseField="0" baseItem="0"/>
+    <dataField name="Duration " fld="4" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Project" xr10:uid="{67259FD2-1E7C-4EC4-8B26-4EAF663DF469}" sourceName="Project">
   <pivotTables>
@@ -10917,17 +9646,17 @@
     <tableColumn id="1" xr3:uid="{4ADE78FA-797E-461B-818D-4E6F917859D6}" name="Project"/>
     <tableColumn id="2" xr3:uid="{F9E92030-47E5-4A86-AB73-A1AA5209CD55}" name="Task"/>
     <tableColumn id="3" xr3:uid="{643837EC-0E87-4517-8311-405E12C9047D}" name="Manager"/>
-    <tableColumn id="4" xr3:uid="{D2195ACD-57B1-4029-9C54-9ACCE862FA18}" name="Start Date" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{D2195ACD-57B1-4029-9C54-9ACCE862FA18}" name="Start Date" dataDxfId="105"/>
     <tableColumn id="5" xr3:uid="{A5BEB9B6-A13C-4735-8C93-943512962E1A}" name="Duration"/>
-    <tableColumn id="9" xr3:uid="{9A8390CA-408A-41FE-A909-4D1F9E77E3F2}" name="End Date" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{9A8390CA-408A-41FE-A909-4D1F9E77E3F2}" name="End Date" dataDxfId="104">
       <calculatedColumnFormula>WORKDAY.INTL(Table1[[#This Row],[Start Date]]-1,Table1[[#This Row],[Duration]],1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{06B5F73C-C916-4EC2-88F2-098623EC6F35}" name="Days completed" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{704AC253-E86F-4A7F-BD63-4569C494A728}" name="Progress" dataDxfId="2" dataCellStyle="Percent">
+    <tableColumn id="10" xr3:uid="{06B5F73C-C916-4EC2-88F2-098623EC6F35}" name="Days completed" dataDxfId="103"/>
+    <tableColumn id="6" xr3:uid="{704AC253-E86F-4A7F-BD63-4569C494A728}" name="Progress" dataDxfId="102" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[Days completed]]/Table1[[#This Row],[Duration]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{459C1C51-A35C-450A-B0F0-EA7E00C33AA1}" name="Budget" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{CC94112E-5637-4797-9BDD-BFCC8197D1AB}" name="Actual" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{459C1C51-A35C-450A-B0F0-EA7E00C33AA1}" name="Budget" dataDxfId="101"/>
+    <tableColumn id="8" xr3:uid="{CC94112E-5637-4797-9BDD-BFCC8197D1AB}" name="Actual" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11237,7 +9966,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK27" sqref="AK27"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12259,7 +10988,7 @@
     <row r="30" spans="1:22" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C30" t="s">
         <v>21</v>
@@ -12561,7 +11290,7 @@
     <row r="40" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
         <v>21</v>
@@ -13111,7 +11840,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K5:AQ5">
-    <cfRule type="expression" dxfId="61" priority="7">
+    <cfRule type="expression" dxfId="161" priority="7">
       <formula>K$5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13130,19 +11859,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:AJ51">
-    <cfRule type="expression" dxfId="60" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="160" priority="1" stopIfTrue="1">
       <formula>$A6="Grand Total"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="159" priority="2" stopIfTrue="1">
       <formula>AND(WEEKDAY(K$5,2)&gt;5,$B6&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="3">
+    <cfRule type="expression" dxfId="158" priority="3">
       <formula>AND(K$5&gt;=$D6,WORKDAY.INTL($D6,$G6,1)-1&gt;=K$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="157" priority="5" stopIfTrue="1">
       <formula>AND(K$5&gt;=WORKDAY.INTL($D6,$G6,1),$H6=0,K$5&lt;=$E6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="6">
+    <cfRule type="expression" dxfId="156" priority="6">
       <formula>AND(K$5&gt;=WORKDAY.INTL($D6,$G6,1),$H6&lt;&gt;1,K$5&lt;=$E6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13209,7 +11938,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13420,8 +12149,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D244"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView showGridLines="0" topLeftCell="A232" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G265" sqref="G265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -13546,7 +12275,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B83" s="38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -13554,7 +12283,7 @@
         <v>63</v>
       </c>
       <c r="B85" s="38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -13567,7 +12296,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B102" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -13593,7 +12322,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B124" s="45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
@@ -13601,7 +12330,7 @@
         <v>71</v>
       </c>
       <c r="B126" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
@@ -13675,62 +12404,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A235BC8-842E-409C-8DB7-81E4CBB62C43}">
-  <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:U18"/>
-  <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-    </row>
-    <row r="2" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="C3" s="53"/>
-    </row>
-    <row r="7" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="N7" s="52"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N9" s="54"/>
-    </row>
-    <row r="18" ht="34.5" customHeight="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA831F74-5EFF-4E8A-B22B-18A2CB322995}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:L41"/>
@@ -14105,7 +12778,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -14455,7 +13128,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C21" t="s">
         <v>21</v>

</xml_diff>